<commit_message>
Determined parameters of the project
Worked out Design Paradigm, Software Architecture, and Design Patterns. Updated hours and gave estimate of total required person hours.
</commit_message>
<xml_diff>
--- a/Documentation/Timesheet.xlsx
+++ b/Documentation/Timesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbthi\Documents\GitHub\EECS-448_Project-3_G11\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panda\Desktop\EECS_448\EECS-448_Project-3_G11\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C085B5-6211-4DD5-A178-BE28197AE47B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3609AED-A036-4E5C-8D5F-39AFB3C05A53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5790" yWindow="720" windowWidth="21600" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -533,15 +533,15 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="8" width="10.44140625" customWidth="1"/>
+    <col min="2" max="8" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
@@ -567,7 +567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
       <c r="B2" s="3">
         <v>44487</v>
@@ -591,7 +591,7 @@
         <v>44493</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -601,11 +601,13 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="F3" s="9">
+        <v>2</v>
+      </c>
       <c r="G3" s="9"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -615,11 +617,13 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="F4" s="10">
+        <v>2</v>
+      </c>
       <c r="G4" s="10"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -629,11 +633,13 @@
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="F5" s="9">
+        <v>2</v>
+      </c>
       <c r="G5" s="9"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -643,11 +649,13 @@
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="F6" s="10">
+        <v>2</v>
+      </c>
       <c r="G6" s="10"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -657,11 +665,13 @@
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+      <c r="F7" s="9">
+        <v>2</v>
+      </c>
       <c r="G7" s="9"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="4">
         <v>44494</v>
@@ -685,7 +695,7 @@
         <v>44500</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -697,7 +707,7 @@
       <c r="G9" s="9"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -709,7 +719,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -721,7 +731,7 @@
       <c r="G11" s="9"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -733,7 +743,7 @@
       <c r="G12" s="10"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
added time for Jigyas
</commit_message>
<xml_diff>
--- a/Documentation/Timesheet.xlsx
+++ b/Documentation/Timesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbthi\Documents\GitHub\EECS-448_Project-3_G11\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stoned_Darksst\Desktop\Fall 2021\EECS 448\Project 2\EECS-448_Project-3_G11\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B39608B-46B5-486C-9C80-3DA7F889E049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C78DA1-9123-46A3-962E-6647EF02496A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -533,15 +533,15 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="8" width="10.44140625" customWidth="1"/>
+    <col min="2" max="8" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
@@ -567,7 +567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
       <c r="B2" s="3">
         <v>44487</v>
@@ -591,7 +591,7 @@
         <v>44493</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -609,25 +609,33 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="7">
         <v>1</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="C4" s="10">
+        <v>2</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0</v>
+      </c>
       <c r="F4" s="10">
         <v>2</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="10">
+        <v>2</v>
+      </c>
       <c r="H4" s="7">
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -645,7 +653,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -661,7 +669,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -679,7 +687,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="4">
         <v>44494</v>
@@ -703,7 +711,7 @@
         <v>44500</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -715,19 +723,23 @@
       <c r="G9" s="9"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="10"/>
+      <c r="B10" s="7">
+        <v>3</v>
+      </c>
+      <c r="C10" s="10">
+        <v>2</v>
+      </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -739,7 +751,7 @@
       <c r="G11" s="9"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -751,7 +763,7 @@
       <c r="G12" s="10"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Added write ups and added more details to other documentation.
</commit_message>
<xml_diff>
--- a/Documentation/Timesheet.xlsx
+++ b/Documentation/Timesheet.xlsx
@@ -1,31 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panda\Desktop\EECS_448\EECS-448_Project-3_G11\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakeangus/Documents/School/Fall_2021/EECS_448/EECS-448_Project-3_G11/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C5FA4B-5884-4414-84A6-EADC8B011158}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36574BC-4CC8-864C-8EAC-8F37795618C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5790" yWindow="720" windowWidth="21600" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5800" yWindow="720" windowWidth="21600" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Sunday</t>
   </si>
@@ -64,13 +95,19 @@
   </si>
   <si>
     <t>Hours Worked</t>
+  </si>
+  <si>
+    <t>Total Person Hours for Project 3:</t>
+  </si>
+  <si>
+    <t>Estimate of Person Hours for Project 3:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,8 +128,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,6 +154,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -211,7 +262,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -247,6 +298,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -530,18 +585,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="8" width="10.42578125" customWidth="1"/>
+    <col min="2" max="8" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="30.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
@@ -567,7 +623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="3">
         <v>44487</v>
@@ -590,8 +646,11 @@
       <c r="H2" s="3">
         <v>44493</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -608,8 +667,11 @@
       <c r="H3" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="15">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -635,7 +697,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -653,7 +715,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -668,8 +730,11 @@
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -686,8 +751,12 @@
       <c r="H7" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J7" s="15" cm="1">
+        <f t="array" ref="J7">SUM(B3:H7+B9:H13)</f>
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="4">
         <v>44494</v>
@@ -711,7 +780,7 @@
         <v>44500</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -723,7 +792,7 @@
       <c r="G9" s="9"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -739,7 +808,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -757,7 +826,7 @@
       <c r="G11" s="9"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -769,7 +838,7 @@
       <c r="G12" s="10"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -785,7 +854,9 @@
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="6"/>
+      <c r="H13" s="6">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added sum on timesheet
</commit_message>
<xml_diff>
--- a/Documentation/Timesheet.xlsx
+++ b/Documentation/Timesheet.xlsx
@@ -1,31 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\GitHub\EECS-448_Project-3_G11\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakeangus/Documents/School/Fall_2021/EECS_448/EECS-448_Project-3_G11/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE68285-3D44-41D4-B0CB-ABB47201249D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAA5CBB-6E4F-5743-92CD-977F725958E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3080" yWindow="1800" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Sunday</t>
   </si>
@@ -64,13 +95,19 @@
   </si>
   <si>
     <t>Hours Worked</t>
+  </si>
+  <si>
+    <t>Estimate of person hours for project 3:</t>
+  </si>
+  <si>
+    <t>Actual Person hours for project 3:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,8 +128,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,6 +154,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -211,7 +262,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -248,6 +299,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -530,18 +589,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="8" width="10.42578125" customWidth="1"/>
+    <col min="2" max="8" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
@@ -567,7 +627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="3">
         <v>44487</v>
@@ -591,7 +651,7 @@
         <v>44493</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -608,8 +668,11 @@
       <c r="H3" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -634,8 +697,11 @@
       <c r="H4" s="7">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" s="14">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -653,7 +719,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -679,7 +745,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -696,8 +762,11 @@
       <c r="H7" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J7" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="4">
         <v>44494</v>
@@ -720,8 +789,12 @@
       <c r="H8" s="4">
         <v>44500</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" s="17" cm="1">
+        <f t="array" ref="J8">SUM(B3:H7+B9:H13)</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -733,7 +806,7 @@
       <c r="G9" s="9"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -749,7 +822,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -773,7 +846,7 @@
       </c>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -799,7 +872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -815,7 +888,9 @@
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="6"/>
+      <c r="H13" s="6">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Minor writing improvements to rules document
</commit_message>
<xml_diff>
--- a/Documentation/Timesheet.xlsx
+++ b/Documentation/Timesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\GitHub\EECS-448_Project-4_G11\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panda\Desktop\EECS_448\EECS-448_Project-4_G11\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D43FCE-B9E8-4D91-BE85-D2883E3CA158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5F3819-B1C6-47EC-919F-D5D8DDC63A76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5790" yWindow="720" windowWidth="21600" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="J22" s="15" cm="1">
         <f t="array" ref="J22">SUM(B17:H21+B23:H27+B29:H33)</f>
-        <v>15.5</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1189,7 +1189,9 @@
       <c r="B31" s="6">
         <v>0.5</v>
       </c>
-      <c r="C31" s="9"/>
+      <c r="C31" s="9">
+        <v>3</v>
+      </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
     </row>

</xml_diff>